<commit_message>
change PartCode to BOM#
</commit_message>
<xml_diff>
--- a/Presentation/Casa.API/FormatFiles/Template_QCAccessory.xlsx
+++ b/Presentation/Casa.API/FormatFiles/Template_QCAccessory.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
-    <t>PartCode</t>
-  </si>
-  <si>
     <t>AccessoryBOMNumber</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>IsActive</t>
+  </si>
+  <si>
+    <t>BOM#</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -439,45 +439,45 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -485,22 +485,22 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>

</xml_diff>